<commit_message>
Labels half way through
</commit_message>
<xml_diff>
--- a/labels.xlsx
+++ b/labels.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18825" windowHeight="12165"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12075" windowHeight="9600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="63">
   <si>
     <t>Sensor</t>
   </si>
@@ -173,9 +173,6 @@
     <t>DampeningConstant</t>
   </si>
   <si>
-    <t>Constant</t>
-  </si>
-  <si>
     <t>SpringSupport</t>
   </si>
   <si>
@@ -194,9 +191,6 @@
     <t>GravityWell</t>
   </si>
   <si>
-    <t>Connect this node to the gravitywell with GravityLabel with afield</t>
-  </si>
-  <si>
     <t>Just variation in calculateforce</t>
   </si>
   <si>
@@ -204,6 +198,21 @@
   </si>
   <si>
     <t>Variations in updateposition</t>
+  </si>
+  <si>
+    <t>Connect this node to the gravitywell with GravityLabel with a field</t>
+  </si>
+  <si>
+    <t>Stationary</t>
+  </si>
+  <si>
+    <t>NodeAngle</t>
+  </si>
+  <si>
+    <t>Visual</t>
+  </si>
+  <si>
+    <t>Colour</t>
   </si>
 </sst>
 </file>
@@ -538,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:F11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,7 +604,7 @@
         <v>31</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -666,7 +675,7 @@
         <v>33</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -802,13 +811,13 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" t="s">
         <v>50</v>
       </c>
-      <c r="D28" t="s">
-        <v>51</v>
-      </c>
       <c r="F28" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -816,7 +825,7 @@
         <v>14</v>
       </c>
       <c r="B29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F29" s="3"/>
     </row>
@@ -825,17 +834,11 @@
         <v>19</v>
       </c>
       <c r="B30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F30" s="3"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31" t="s">
-        <v>27</v>
-      </c>
       <c r="F31" s="3"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -845,9 +848,6 @@
       <c r="B32" t="s">
         <v>1</v>
       </c>
-      <c r="D32" t="s">
-        <v>49</v>
-      </c>
       <c r="F32" s="3"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -867,24 +867,52 @@
         <v>17</v>
       </c>
       <c r="B34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F34" s="3"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>53</v>
-      </c>
-      <c r="D36" t="s">
-        <v>54</v>
-      </c>
-      <c r="F36" t="s">
-        <v>56</v>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>55</v>
+        <v>52</v>
+      </c>
+      <c r="D37" t="s">
+        <v>53</v>
+      </c>
+      <c r="F37" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
redoing creation to handle Labels instead of args
</commit_message>
<xml_diff>
--- a/labels.xlsx
+++ b/labels.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12075" windowHeight="9600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2280" windowHeight="8790"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="77">
   <si>
     <t>Sensor</t>
   </si>
@@ -107,9 +107,6 @@
     <t>Sensor, Node</t>
   </si>
   <si>
-    <t>PullSpring, PushSpring</t>
-  </si>
-  <si>
     <t>BinaryActuator</t>
   </si>
   <si>
@@ -158,9 +155,6 @@
     <t>NodeCollectionPicture</t>
   </si>
   <si>
-    <t xml:space="preserve">Scale, </t>
-  </si>
-  <si>
     <t>Picture, CollectionNode</t>
   </si>
   <si>
@@ -173,9 +167,6 @@
     <t>DampeningConstant</t>
   </si>
   <si>
-    <t>SpringSupport</t>
-  </si>
-  <si>
     <t>Constant, EquilibriumLength</t>
   </si>
   <si>
@@ -191,9 +182,6 @@
     <t>GravityWell</t>
   </si>
   <si>
-    <t>Just variation in calculateforce</t>
-  </si>
-  <si>
     <t>Just variations in updateposition, sense and show with some supportfunctions and constructorvariations</t>
   </si>
   <si>
@@ -203,9 +191,6 @@
     <t>Connect this node to the gravitywell with GravityLabel with a field</t>
   </si>
   <si>
-    <t>Stationary</t>
-  </si>
-  <si>
     <t>NodeAngle</t>
   </si>
   <si>
@@ -213,13 +198,144 @@
   </si>
   <si>
     <t>Colour</t>
+  </si>
+  <si>
+    <t>Angle, Torque Constant,</t>
+  </si>
+  <si>
+    <t>Movable</t>
+  </si>
+  <si>
+    <t>Mass, Node friction</t>
+  </si>
+  <si>
+    <t>truss</t>
+  </si>
+  <si>
+    <r>
+      <t>screenSize</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>worldSize</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>setWorldOffset</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>fpsTarget</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>fps</t>
+    </r>
+  </si>
+  <si>
+    <t>node</t>
+  </si>
+  <si>
+    <t>parent</t>
+  </si>
+  <si>
+    <t>NodeDebug</t>
+  </si>
+  <si>
+    <t>Angle</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Size, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Velocity, CurrentLength, turnrate, </t>
+  </si>
+  <si>
+    <t>Angle, torqueConstant</t>
+  </si>
+  <si>
+    <t>VelocityBasedTensors, PositionBasedTensors</t>
+  </si>
+  <si>
+    <t>positionFunction, showFunction</t>
+  </si>
+  <si>
+    <t>Visible</t>
+  </si>
+  <si>
+    <t>Tensor, Hidden</t>
+  </si>
+  <si>
+    <t>Hidden</t>
+  </si>
+  <si>
+    <t>Tensor, -Hidden</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,6 +356,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Fira Code"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9CDCFE"/>
+      <name val="Fira Code"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -262,11 +390,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,334 +723,402 @@
       <c r="B4" t="s">
         <v>3</v>
       </c>
+      <c r="D4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
       <c r="D6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
       <c r="D7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="3"/>
+        <v>72</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="3"/>
+        <v>30</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
       </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
       <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>56</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D13" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
         <v>2</v>
       </c>
-      <c r="D14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="F15" s="3"/>
+      <c r="D15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" t="s">
-        <v>0</v>
-      </c>
+      <c r="A18" s="1"/>
       <c r="F18" s="3"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B19" t="s">
         <v>26</v>
       </c>
+      <c r="D19" t="s">
+        <v>35</v>
+      </c>
       <c r="F19" s="3"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B20" t="s">
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F20" s="3"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
+      <c r="A21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F21" s="3"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B25" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>41</v>
-      </c>
-      <c r="B24" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>43</v>
-      </c>
-      <c r="B25" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>42</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" t="s">
         <v>18</v>
       </c>
-      <c r="D26" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D28" t="s">
-        <v>50</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" t="s">
-        <v>49</v>
-      </c>
-      <c r="F29" s="3"/>
+      <c r="D29" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B30" t="s">
-        <v>49</v>
-      </c>
-      <c r="F30" s="3"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F31" s="3"/>
+      <c r="A30" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>15</v>
+      <c r="A32" t="s">
+        <v>66</v>
       </c>
       <c r="B32" t="s">
-        <v>1</v>
-      </c>
-      <c r="F32" s="3"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B33" t="s">
-        <v>1</v>
-      </c>
-      <c r="D33" t="s">
-        <v>48</v>
-      </c>
-      <c r="F33" s="3"/>
+        <v>63</v>
+      </c>
+      <c r="D32" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B34" t="s">
-        <v>51</v>
-      </c>
-      <c r="F34" s="3"/>
+        <v>76</v>
+      </c>
+      <c r="D34" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B35" t="s">
-        <v>27</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="D35" t="s">
+        <v>47</v>
+      </c>
+      <c r="F35" s="3"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" t="s">
+        <v>76</v>
+      </c>
+      <c r="D36" t="s">
+        <v>47</v>
+      </c>
+      <c r="F36" s="3"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>52</v>
-      </c>
-      <c r="D37" t="s">
-        <v>53</v>
-      </c>
-      <c r="F37" t="s">
-        <v>58</v>
-      </c>
+      <c r="F37" s="3"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="A38" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38" t="s">
+        <v>74</v>
+      </c>
+      <c r="F38" s="3"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" t="s">
+        <v>74</v>
+      </c>
+      <c r="D39" t="s">
+        <v>46</v>
+      </c>
+      <c r="F39" s="3"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B40" t="s">
+        <v>48</v>
+      </c>
+      <c r="F40" s="3"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>49</v>
+      </c>
+      <c r="D42" t="s">
+        <v>50</v>
+      </c>
+      <c r="F42" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>59</v>
+      </c>
+      <c r="D45" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>55</v>
+      </c>
+      <c r="D46" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="B53" t="s">
+        <v>63</v>
+      </c>
+      <c r="D53" s="4" t="s">
         <v>62</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="F28:F34"/>
-    <mergeCell ref="F12:F20"/>
-    <mergeCell ref="F6:F11"/>
+    <mergeCell ref="F35:F40"/>
+    <mergeCell ref="F15:F23"/>
+    <mergeCell ref="F9:F14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>